<commit_message>
NacAuto Login\Register Positive Tests implementation
</commit_message>
<xml_diff>
--- a/Test Cases/Positive Test Cases/Log in Test Suite.xlsx
+++ b/Test Cases/Positive Test Cases/Log in Test Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -82,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +182,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,17 +391,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -456,7 +459,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>